<commit_message>
fix(upload_drive.js) and fix(select all)
</commit_message>
<xml_diff>
--- a/server/LISTAS/ma/BURLETES AUTOADHESIVOS DISMAY.xlsx
+++ b/server/LISTAS/ma/BURLETES AUTOADHESIVOS DISMAY.xlsx
@@ -731,7 +731,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="23" t="n">
-        <v>45302</v>
+        <v>45308</v>
       </c>
       <c r="E1" s="5" t="n"/>
     </row>
@@ -954,19 +954,19 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A1:D1"/>
     <mergeCell ref="B38:C38"/>
+    <mergeCell ref="A9:D9"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B37:C37"/>
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B32:C32"/>
     <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="A10:D10"/>
     <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="B36:C36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>